<commit_message>
feat: new MID bot close to finish
</commit_message>
<xml_diff>
--- a/04 - MID/03 - Delete/01 - Demand/Data.xlsx
+++ b/04 - MID/03 - Delete/01 - Demand/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\04 - MID\03 - Delete\01 - Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E6A21-396A-4AF9-87DD-382DF97008F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3613A-885A-4424-94C3-5AB89D27520E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{841C4129-0CB3-4066-B34E-E8845E3509BE}"/>
   </bookViews>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D997F1F-30FE-4A2A-B694-A9178A4FC344}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A39"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,191 +443,186 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>685601396368</v>
+        <v>685601396367</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>685601396367</v>
+        <v>685601396366</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>685601396366</v>
+        <v>685601396364</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>685601396364</v>
+        <v>685601396363</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>685601396363</v>
+        <v>685601396361</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>685601396361</v>
+        <v>685601395673</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>685601395673</v>
+        <v>685601395672</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>685601395672</v>
+        <v>685601395664</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>685601395664</v>
+        <v>685601395653</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>685601395653</v>
+        <v>685601395652</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>685601395652</v>
+        <v>685601395651</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>685601395651</v>
+        <v>685601395650</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>685601395650</v>
+        <v>685601395649</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>685601395649</v>
+        <v>685601395647</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>685601395647</v>
+        <v>685601395646</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>685601395646</v>
+        <v>685601394437</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>685601394437</v>
+        <v>685601394435</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>685601394435</v>
+        <v>685601394434</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>685601394434</v>
+        <v>685601394433</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>685601394433</v>
+        <v>685601394430</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>685601394430</v>
+        <v>685601394429</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>685601394429</v>
+        <v>685601394428</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>685601394428</v>
+        <v>685601394427</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>685601394427</v>
+        <v>685601394426</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>685601394426</v>
+        <v>685601394425</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>685601394425</v>
+        <v>685601394354</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>685601394354</v>
+        <v>685601392511</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>685601392511</v>
+        <v>685601391111</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>685601391111</v>
+        <v>685601389719</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>685601389719</v>
+        <v>685601388006</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>685601388006</v>
+        <v>685601385430</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>685601385430</v>
+        <v>685601385337</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>685601385337</v>
+        <v>685601383707</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>685601383707</v>
+        <v>685601382486</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>685601382486</v>
+        <v>685601382483</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>685601382483</v>
+        <v>685601382481</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>685601382481</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
         <v>685601381735</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: bot to finish demand is complete
</commit_message>
<xml_diff>
--- a/04 - MID/03 - Delete/01 - Demand/Data.xlsx
+++ b/04 - MID/03 - Delete/01 - Demand/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\04 - MID\03 - Delete\01 - Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3613A-885A-4424-94C3-5AB89D27520E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5340258A-30FF-4A58-B3E8-27FE69EC78DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{841C4129-0CB3-4066-B34E-E8845E3509BE}"/>
   </bookViews>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D997F1F-30FE-4A2A-B694-A9178A4FC344}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,186 +443,136 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>685601396367</v>
+        <v>685601395651</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>685601396366</v>
+        <v>685601395650</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>685601396364</v>
+        <v>685601395649</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>685601396363</v>
+        <v>685601395647</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>685601396361</v>
+        <v>685601395646</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>685601395673</v>
+        <v>685601394437</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>685601395672</v>
+        <v>685601394435</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>685601395664</v>
+        <v>685601394434</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>685601395653</v>
+        <v>685601394433</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>685601395652</v>
+        <v>685601394430</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>685601395651</v>
+        <v>685601394429</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>685601395650</v>
+        <v>685601394428</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>685601395649</v>
+        <v>685601394427</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>685601395647</v>
+        <v>685601394426</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>685601395646</v>
+        <v>685601394425</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>685601394437</v>
+        <v>685601394354</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>685601394435</v>
+        <v>685601392511</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>685601394434</v>
+        <v>685601391111</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>685601394433</v>
+        <v>685601389719</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>685601394430</v>
+        <v>685601388006</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>685601394429</v>
+        <v>685601385430</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>685601394428</v>
+        <v>685601385337</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>685601394427</v>
+        <v>685601383707</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>685601394426</v>
+        <v>685601382486</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>685601394425</v>
+        <v>685601382483</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>685601394354</v>
+        <v>685601382481</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>685601392511</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>685601391111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>685601389719</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>685601388006</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>685601385430</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>685601385337</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>685601383707</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>685601382486</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>685601382483</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>685601382481</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
         <v>685601381735</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: updated images, unknown error with prints
</commit_message>
<xml_diff>
--- a/04 - MID/03 - Delete/01 - Demand/Data.xlsx
+++ b/04 - MID/03 - Delete/01 - Demand/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\04 - MID\03 - Delete\01 - Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5340258A-30FF-4A58-B3E8-27FE69EC78DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061B77FF-EC33-4E42-9287-BFAB717D6D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{841C4129-0CB3-4066-B34E-E8845E3509BE}"/>
   </bookViews>
@@ -103,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,6 +111,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D997F1F-30FE-4A2A-B694-A9178A4FC344}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A28"/>
+      <selection activeCell="F6" sqref="F6:V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,145 +437,147 @@
     <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>685601395651</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>685601395650</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>685601395649</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397704</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>685601395647</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>685601395646</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>685601394437</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>685601394435</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397699</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>685601394434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397698</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>685601394433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397697</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>685601394430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397696</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>685601394429</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397695</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>685601394428</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397694</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>685601394427</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>685601397692</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>685601394426</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>685601394425</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>685601394354</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>685601392511</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>685601391111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>685601389719</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>685601388006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>685601385430</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>685601385337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>685601383707</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>685601382486</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>685601382483</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>685601382481</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>685601381735</v>
-      </c>
+        <v>685601397691</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>